<commit_message>
Correcao do texto Nome da mae ou responsavel no arquivo padrao xls para download
</commit_message>
<xml_diff>
--- a/public/downloads/padrao_importacao.xlsx
+++ b/public/downloads/padrao_importacao.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansouza\Documents\www\arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansouza\Documents\www\busca-ativa-escolar-lp\public\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0123CE2F-00E3-4C15-A5B6-015E55EEF5E8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A507C885-B17B-49E0-BA8E-6D1F684D59DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CFB3E84B-36E1-41B0-A2CE-7A4B023401E0}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>Data de nascimento</t>
   </si>
   <si>
-    <t>Nome da mãe</t>
-  </si>
-  <si>
     <t>Nome do pai</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>Observações</t>
+  </si>
+  <si>
+    <t>Nome da mãe ou responsável</t>
   </si>
 </sst>
 </file>
@@ -422,14 +422,15 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="11" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -440,31 +441,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>